<commit_message>
Updated Cat Map and Card Data
</commit_message>
<xml_diff>
--- a/NearlineSupervisedRecommendationGenerator/Cat_Map.xlsx
+++ b/NearlineSupervisedRecommendationGenerator/Cat_Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52jai\Python\Intern\Current Work\Latest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52jai\Python\Intern\Current Work\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40AC764-998A-4F8F-8A2B-52C0AE5706B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00904AE0-C6B9-4C70-902A-F0E1F55D70C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="2760" windowWidth="21600" windowHeight="11835" xr2:uid="{3965857F-0777-4097-A372-BACCA0C46172}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3965857F-0777-4097-A372-BACCA0C46172}"/>
   </bookViews>
   <sheets>
     <sheet name="CategoryMap" sheetId="1" r:id="rId1"/>
@@ -451,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14800B0-FB80-4AD3-BEEB-BC770582263E}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +520,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H2" s="1">
         <v>2</v>
@@ -680,7 +680,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
@@ -712,7 +712,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H8" s="1">
         <v>8</v>
@@ -744,7 +744,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H9" s="1">
         <v>5</v>
@@ -808,7 +808,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H11" s="1">
         <v>2</v>
@@ -872,7 +872,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H13" s="1">
         <v>2</v>
@@ -927,7 +927,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -1011,6 +1011,17 @@
       <c r="J17" s="1">
         <v>0</v>
       </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>